<commit_message>
dialogs done for 30 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/TwoThousands.xlsx
+++ b/public/docs/Excel data/TwoThousands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195CF26A-3B51-4CBF-9FB9-D220795B737B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3628A73B-11DD-482F-B564-4261742700B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11503" uniqueCount="4862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11593" uniqueCount="4952">
   <si>
     <t>з</t>
   </si>
@@ -14628,13 +14628,283 @@
   </si>
   <si>
     <t>🪧 10. HELP WANTED / NOW HIRING</t>
+  </si>
+  <si>
+    <t>//LESSON 10</t>
+  </si>
+  <si>
+    <t>//LESSON 11</t>
+  </si>
+  <si>
+    <t>//LESSON 12</t>
+  </si>
+  <si>
+    <t>//LESSON 13</t>
+  </si>
+  <si>
+    <t>//LESSON 14</t>
+  </si>
+  <si>
+    <t>//LESSON 15</t>
+  </si>
+  <si>
+    <t>//LESSON 16</t>
+  </si>
+  <si>
+    <t>//LESSON 17</t>
+  </si>
+  <si>
+    <t>//LESSON 18</t>
+  </si>
+  <si>
+    <t>//LESSON 19</t>
+  </si>
+  <si>
+    <t>//LESSON 20</t>
+  </si>
+  <si>
+    <t>//LESSON 21</t>
+  </si>
+  <si>
+    <t>//LESSON 22</t>
+  </si>
+  <si>
+    <t>//LESSON 23</t>
+  </si>
+  <si>
+    <t>//LESSON 24</t>
+  </si>
+  <si>
+    <t>//LESSON 25</t>
+  </si>
+  <si>
+    <t>//LESSON 26</t>
+  </si>
+  <si>
+    <t>//LESSON 27</t>
+  </si>
+  <si>
+    <t>//LESSON 28</t>
+  </si>
+  <si>
+    <t>//LESSON 30</t>
+  </si>
+  <si>
+    <t>Books &amp; Reading – Talk about favorite books, authors, or reading habits.</t>
+  </si>
+  <si>
+    <t>Pets &amp; Animals – Discuss experiences with pets, favorite animals, or wildlife encounters.</t>
+  </si>
+  <si>
+    <t>Environment &amp; Nature – Share views on environmental issues, nature walks, or sustainable living.</t>
+  </si>
+  <si>
+    <t>Hometown &amp; Neighborhood – Describe where you live or grew up, and what makes it special.</t>
+  </si>
+  <si>
+    <t>Languages &amp; Communication – Talk about languages you know, want to learn, or language barriers.</t>
+  </si>
+  <si>
+    <t>Fashion &amp; Style – Discuss clothing preferences, trends, and personal style.</t>
+  </si>
+  <si>
+    <t>Celebrations &amp; Festivals – Share traditions around birthdays, holidays, and national celebrations.</t>
+  </si>
+  <si>
+    <t>Art &amp; Creativity – Talk about drawing, painting, design, or any creative projects you enjoy.</t>
+  </si>
+  <si>
+    <t>Transportation &amp; Commuting – Describe how you get around and experiences with travel or commuting.</t>
+  </si>
+  <si>
+    <t>Challenges &amp; Achievements – Reflect on personal obstacles and proud accomplishments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introductions &amp; Personal Information </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about yourself, your background, and your interests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily Routines </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Describe your typical day from morning to night.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobbies &amp; Free Time </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss your favorite activities, sports, or creative pursuits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel &amp; Holidays </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Share experiences about past trips or dream destinations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food &amp; Cooking </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about favorite dishes, recipes, and eating habits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family &amp; Friends </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Describe your relationships and social life.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School &amp; Education </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss school experiences, favorite subjects, and learning methods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work &amp; Careers </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about jobs, career goals, and workplace culture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shopping &amp; Money </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss buying habits, budgeting, and favorite stores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technology &amp; Social Media </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about how you use technology and its effects on daily life.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movies &amp; TV Shows </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Share opinions on films, series, and actors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music &amp; Entertainment </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about favorite musicians, concerts, and music genres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sports &amp; Exercise </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss favorite sports, fitness routines, and staying healthy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News &amp; Current Events </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Share thoughts on recent world events and local news.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dreams &amp; Future Plans </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about life goals, ambitions, and hopes for the future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cultural Differences </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss traditions, customs, and cultural experiences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather &amp; Seasons </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about favorite seasons and how weather affects daily life.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health &amp; Wellness </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss habits for staying healthy and dealing with stress.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Experiences &amp; Stories </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Share interesting life events or funny stories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If You Could... </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Imagine different scenarios like "If you could travel anywhere, where would you go?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Books &amp; Reading </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about favorite books, authors, or reading habits.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pets &amp; Animals </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss experiences with pets, favorite animals, or wildlife encounters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment &amp; Nature </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Share views on environmental issues, nature walks, or sustainable living.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hometown &amp; Neighborhood </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Describe where you live or grew up, and what makes it special.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages &amp; Communication </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about languages you know, want to learn, or language barriers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fashion &amp; Style </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discuss clothing preferences, trends, and personal style.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celebrations &amp; Festivals </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Share traditions around birthdays, holidays, and national celebrations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Art &amp; Creativity </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Talk about drawing, painting, design, or any creative projects you enjoy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation &amp; Commuting </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Describe how you get around and experiences with travel or commuting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Challenges &amp; Achievements </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reflect on personal obstacles and proud accomplishments.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14668,6 +14938,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -14720,7 +14996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -14736,6 +15012,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72071,184 +72351,508 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E59B5-B434-461C-8003-542FC86AE77F}">
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="98.33203125" customWidth="1"/>
+    <col min="4" max="4" width="77.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>4773</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>4774</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>4892</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4893</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>4775</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>4894</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4895</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>4776</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>4896</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4897</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>4777</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>4898</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4899</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>4863</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>4778</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>4900</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4901</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>4864</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>4779</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>4902</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4903</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>4865</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>4780</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>4904</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4905</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>4866</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>4781</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>4906</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4907</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>4867</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>4782</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>4908</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4909</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>4868</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>4783</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>4910</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4911</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>4869</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>4784</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>4912</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4913</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>4870</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>4785</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>4914</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4915</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>4871</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>4786</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>4916</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4917</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>4872</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>4787</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>4918</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4919</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>4873</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>4788</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>4920</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4921</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>4874</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>4789</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>4922</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4923</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>4875</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>4790</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>4924</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4925</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>4876</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>4791</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>4926</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4927</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>4877</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>4792</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>4928</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4929</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>4878</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>4793</v>
       </c>
+      <c r="D22" t="s">
+        <v>4930</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4931</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>4879</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>4882</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>4932</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4933</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>4880</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>4883</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>4934</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4935</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>4881</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>4884</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>4936</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4937</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>4885</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>4938</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4939</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>4886</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>4940</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4941</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>4887</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>4942</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4943</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>4888</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>4944</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4945</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>4889</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>4946</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4947</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>4890</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>4948</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4949</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>4891</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>4950</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4951</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -72644,7 +73248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F62D7B-A016-4862-8D3B-A22E04A436CB}">
   <dimension ref="B2:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
speaking text done for 5 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/TwoThousands.xlsx
+++ b/public/docs/Excel data/TwoThousands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3628A73B-11DD-482F-B564-4261742700B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ADAEFB-44C6-47ED-A7DF-20E121646F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="11016" yWindow="384" windowWidth="11760" windowHeight="8880" activeTab="4" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11593" uniqueCount="4952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11653" uniqueCount="5012">
   <si>
     <t>з</t>
   </si>
@@ -14898,6 +14898,186 @@
   </si>
   <si>
     <t xml:space="preserve"> Reflect on personal obstacles and proud accomplishments.</t>
+  </si>
+  <si>
+    <t>// LESSON 1</t>
+  </si>
+  <si>
+    <t>// Introductions &amp; Personal Information</t>
+  </si>
+  <si>
+    <t>// LESSON 2</t>
+  </si>
+  <si>
+    <t>// Daily Routines</t>
+  </si>
+  <si>
+    <t>// LESSON 3</t>
+  </si>
+  <si>
+    <t>// Hobbies &amp; Free Time</t>
+  </si>
+  <si>
+    <t>// LESSON 4</t>
+  </si>
+  <si>
+    <t>// Travel &amp; Holidays</t>
+  </si>
+  <si>
+    <t>// LESSON 5</t>
+  </si>
+  <si>
+    <t>// Food &amp; Cooking</t>
+  </si>
+  <si>
+    <t>// LESSON 6</t>
+  </si>
+  <si>
+    <t>// Family &amp; Friends</t>
+  </si>
+  <si>
+    <t>// LESSON 7</t>
+  </si>
+  <si>
+    <t>// School &amp; Education</t>
+  </si>
+  <si>
+    <t>// LESSON 8</t>
+  </si>
+  <si>
+    <t>// Work &amp; Careers</t>
+  </si>
+  <si>
+    <t>// LESSON 9</t>
+  </si>
+  <si>
+    <t>// Shopping &amp; Money</t>
+  </si>
+  <si>
+    <t>// LESSON 10</t>
+  </si>
+  <si>
+    <t>// Technology &amp; Social Media</t>
+  </si>
+  <si>
+    <t>// LESSON 11</t>
+  </si>
+  <si>
+    <t>// Movies &amp; TV Shows</t>
+  </si>
+  <si>
+    <t>// LESSON 12</t>
+  </si>
+  <si>
+    <t>// Music &amp; Entertainment</t>
+  </si>
+  <si>
+    <t>// LESSON 13</t>
+  </si>
+  <si>
+    <t>// Sports &amp; Exercise</t>
+  </si>
+  <si>
+    <t>// LESSON 14</t>
+  </si>
+  <si>
+    <t>// News &amp; Current Events</t>
+  </si>
+  <si>
+    <t>// LESSON 15</t>
+  </si>
+  <si>
+    <t>// Dreams &amp; Future Plans</t>
+  </si>
+  <si>
+    <t>// LESSON 16</t>
+  </si>
+  <si>
+    <t>// Cultural Differences</t>
+  </si>
+  <si>
+    <t>// LESSON 17</t>
+  </si>
+  <si>
+    <t>// Weather &amp; Seasons</t>
+  </si>
+  <si>
+    <t>// LESSON 18</t>
+  </si>
+  <si>
+    <t>// Health &amp; Wellness</t>
+  </si>
+  <si>
+    <t>// LESSON 19</t>
+  </si>
+  <si>
+    <t>// Personal Experiences &amp; Stories</t>
+  </si>
+  <si>
+    <t>// LESSON 20</t>
+  </si>
+  <si>
+    <t>// If You Could...</t>
+  </si>
+  <si>
+    <t>// LESSON 21</t>
+  </si>
+  <si>
+    <t>// Books &amp; Reading</t>
+  </si>
+  <si>
+    <t>// LESSON 22</t>
+  </si>
+  <si>
+    <t>// Pets &amp; Animals</t>
+  </si>
+  <si>
+    <t>// LESSON 23</t>
+  </si>
+  <si>
+    <t>// Environment &amp; Nature</t>
+  </si>
+  <si>
+    <t>// LESSON 24</t>
+  </si>
+  <si>
+    <t>// Hometown &amp; Neighborhood</t>
+  </si>
+  <si>
+    <t>// LESSON 25</t>
+  </si>
+  <si>
+    <t>// Languages &amp; Communication</t>
+  </si>
+  <si>
+    <t>// LESSON 26</t>
+  </si>
+  <si>
+    <t>// Fashion &amp; Style</t>
+  </si>
+  <si>
+    <t>// LESSON 27</t>
+  </si>
+  <si>
+    <t>// Celebrations &amp; Festivals</t>
+  </si>
+  <si>
+    <t>// LESSON 28</t>
+  </si>
+  <si>
+    <t>// Art &amp; Creativity</t>
+  </si>
+  <si>
+    <t>// LESSON 29</t>
+  </si>
+  <si>
+    <t>// Transportation &amp; Commuting</t>
+  </si>
+  <si>
+    <t>// LESSON 30</t>
+  </si>
+  <si>
+    <t>// Challenges &amp; Achievements</t>
   </si>
 </sst>
 </file>
@@ -14996,7 +15176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -15015,7 +15195,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72351,25 +72530,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E59B5-B434-461C-8003-542FC86AE77F}">
-  <dimension ref="B2:G32"/>
+  <dimension ref="B2:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="98.33203125" customWidth="1"/>
-    <col min="4" max="4" width="77.33203125" customWidth="1"/>
-    <col min="7" max="7" width="30.21875" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="6" max="6" width="52.77734375" customWidth="1"/>
+    <col min="7" max="7" width="52.21875" customWidth="1"/>
+    <col min="8" max="8" width="30.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>4773</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -72382,8 +72563,11 @@
       <c r="E3" t="s">
         <v>4893</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>4952</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -72396,8 +72580,11 @@
       <c r="E4" t="s">
         <v>4895</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>4953</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3</v>
       </c>
@@ -72410,11 +72597,11 @@
       <c r="E5" t="s">
         <v>4897</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>4862</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -72427,11 +72614,14 @@
       <c r="E6" t="s">
         <v>4899</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" t="s">
+        <v>4954</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>4863</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -72444,11 +72634,14 @@
       <c r="E7" t="s">
         <v>4901</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" t="s">
+        <v>4955</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>4864</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6</v>
       </c>
@@ -72461,11 +72654,11 @@
       <c r="E8" t="s">
         <v>4903</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>4865</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>7</v>
       </c>
@@ -72478,11 +72671,14 @@
       <c r="E9" t="s">
         <v>4905</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" t="s">
+        <v>4956</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>4866</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8</v>
       </c>
@@ -72495,11 +72691,14 @@
       <c r="E10" t="s">
         <v>4907</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" t="s">
+        <v>4957</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>4867</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>9</v>
       </c>
@@ -72512,11 +72711,11 @@
       <c r="E11" t="s">
         <v>4909</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>4868</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>10</v>
       </c>
@@ -72529,11 +72728,17 @@
       <c r="E12" t="s">
         <v>4911</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" t="s">
+        <v>4958</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>4869</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>11</v>
       </c>
@@ -72546,11 +72751,14 @@
       <c r="E13" t="s">
         <v>4913</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" t="s">
+        <v>4959</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>4870</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -72563,11 +72771,11 @@
       <c r="E14" t="s">
         <v>4915</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>4871</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>13</v>
       </c>
@@ -72580,11 +72788,14 @@
       <c r="E15" t="s">
         <v>4917</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" t="s">
+        <v>4960</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>4872</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>14</v>
       </c>
@@ -72597,11 +72808,14 @@
       <c r="E16" t="s">
         <v>4919</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" t="s">
+        <v>4961</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>4873</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>15</v>
       </c>
@@ -72614,11 +72828,11 @@
       <c r="E17" t="s">
         <v>4921</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>4874</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>16</v>
       </c>
@@ -72631,11 +72845,14 @@
       <c r="E18" t="s">
         <v>4923</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" t="s">
+        <v>4962</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>4875</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>17</v>
       </c>
@@ -72648,11 +72865,14 @@
       <c r="E19" t="s">
         <v>4925</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" t="s">
+        <v>4963</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>4876</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>18</v>
       </c>
@@ -72665,11 +72885,11 @@
       <c r="E20" t="s">
         <v>4927</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="9" t="s">
         <v>4877</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>19</v>
       </c>
@@ -72682,11 +72902,14 @@
       <c r="E21" t="s">
         <v>4929</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" t="s">
+        <v>4964</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>4878</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>20</v>
       </c>
@@ -72699,154 +72922,375 @@
       <c r="E22" t="s">
         <v>4931</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" t="s">
+        <v>4965</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>4879</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>21</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" t="s">
         <v>4882</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" t="s">
         <v>4932</v>
       </c>
       <c r="E23" t="s">
         <v>4933</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>4880</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>22</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" t="s">
         <v>4883</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" t="s">
         <v>4934</v>
       </c>
       <c r="E24" t="s">
         <v>4935</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" t="s">
+        <v>4966</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>4881</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>23</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" t="s">
         <v>4884</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" t="s">
         <v>4936</v>
       </c>
       <c r="E25" t="s">
         <v>4937</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>4967</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>24</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" t="s">
         <v>4885</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" t="s">
         <v>4938</v>
       </c>
       <c r="E26" t="s">
         <v>4939</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>25</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" t="s">
         <v>4886</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" t="s">
         <v>4940</v>
       </c>
       <c r="E27" t="s">
         <v>4941</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>4968</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>26</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" t="s">
         <v>4887</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" t="s">
         <v>4942</v>
       </c>
       <c r="E28" t="s">
         <v>4943</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>4969</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>27</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" t="s">
         <v>4888</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" t="s">
         <v>4944</v>
       </c>
       <c r="E29" t="s">
         <v>4945</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>28</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" t="s">
         <v>4889</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" t="s">
         <v>4946</v>
       </c>
       <c r="E30" t="s">
         <v>4947</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>4970</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>29</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" t="s">
         <v>4890</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" t="s">
         <v>4948</v>
       </c>
       <c r="E31" t="s">
         <v>4949</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>4971</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>30</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" t="s">
         <v>4891</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" t="s">
         <v>4950</v>
       </c>
       <c r="E32" t="s">
         <v>4951</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>4972</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>4973</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G36" t="s">
+        <v>4974</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>4975</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>4976</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>4977</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>4978</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>4979</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>4980</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>4981</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>4982</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>4983</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>4984</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>4985</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>4986</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>4987</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>4988</v>
+      </c>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>4989</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G60" t="s">
+        <v>4990</v>
+      </c>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G61" t="s">
+        <v>4991</v>
+      </c>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>4992</v>
+      </c>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>4993</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>4994</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G67" t="s">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>4996</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G70" t="s">
+        <v>4997</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G72" t="s">
+        <v>4998</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G73" t="s">
+        <v>4999</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G75" t="s">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G76" t="s">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G78" t="s">
+        <v>5002</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G79" t="s">
+        <v>5003</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G82" t="s">
+        <v>5005</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G84" t="s">
+        <v>5006</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G85" t="s">
+        <v>5007</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G87" t="s">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G88" t="s">
+        <v>5009</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G90" t="s">
+        <v>5010</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G91" t="s">
+        <v>5011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grammar rules completed for 20 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/TwoThousands.xlsx
+++ b/public/docs/Excel data/TwoThousands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ADAEFB-44C6-47ED-A7DF-20E121646F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9366555-173A-472F-B5DA-DBB4F822058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11016" yWindow="384" windowWidth="11760" windowHeight="8880" activeTab="4" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
@@ -71843,8 +71843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065B795-6495-421C-8C31-54BC300F0CEC}">
   <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72532,7 +72532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E59B5-B434-461C-8003-542FC86AE77F}">
   <dimension ref="B2:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+    <sheetView topLeftCell="F2" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replace it completed for 30 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/TwoThousands.xlsx
+++ b/public/docs/Excel data/TwoThousands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9366555-173A-472F-B5DA-DBB4F822058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1B35F5-464F-47B4-BEE9-614890EE4ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="804" yWindow="756" windowWidth="21600" windowHeight="11232" activeTab="7" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Topics" sheetId="9" r:id="rId5"/>
     <sheet name="LessonStructure" sheetId="10" r:id="rId6"/>
     <sheet name="ReadingSigns" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11653" uniqueCount="5012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11716" uniqueCount="5057">
   <si>
     <t>з</t>
   </si>
@@ -15078,13 +15079,252 @@
   </si>
   <si>
     <t>// Challenges &amp; Achievements</t>
+  </si>
+  <si>
+    <t>Іменник (однина)</t>
+  </si>
+  <si>
+    <t>Множина</t>
+  </si>
+  <si>
+    <t>Переклад</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>чоловік – чоловіки</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>жінка – жінки</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>дитина – діти</t>
+  </si>
+  <si>
+    <t>teeth</t>
+  </si>
+  <si>
+    <t>зуб – зуби</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>ступня – ступні</t>
+  </si>
+  <si>
+    <t>mice</t>
+  </si>
+  <si>
+    <t>миша – миші</t>
+  </si>
+  <si>
+    <t>goose</t>
+  </si>
+  <si>
+    <t>geese</t>
+  </si>
+  <si>
+    <t>гуска – гуски</t>
+  </si>
+  <si>
+    <t>особа – люди</t>
+  </si>
+  <si>
+    <t>ox</t>
+  </si>
+  <si>
+    <t>oxen</t>
+  </si>
+  <si>
+    <t>віл – воли</t>
+  </si>
+  <si>
+    <t>louse</t>
+  </si>
+  <si>
+    <t>lice</t>
+  </si>
+  <si>
+    <t>воша – воші</t>
+  </si>
+  <si>
+    <t>sheep</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">вівця – вівці </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <t>deer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">олень – олені </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">риба – риби </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <t>aircraft</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">літак – літаки </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">вид – види </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">серія – серії </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <t>salmon</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">лосось – лососі </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <t>means</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">засіб – засоби </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(незмінне)</t>
+    </r>
+  </si>
+  <si>
+    <t>cactus</t>
+  </si>
+  <si>
+    <t>cacti</t>
+  </si>
+  <si>
+    <t>кактус – кактуси</t>
+  </si>
+  <si>
+    <t>phenomenon</t>
+  </si>
+  <si>
+    <t>phenomena</t>
+  </si>
+  <si>
+    <t>явище – явища</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15124,6 +15364,14 @@
       <color rgb="FF6A9955"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -15176,7 +15424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -15194,6 +15442,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -71843,7 +72097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065B795-6495-421C-8C31-54BC300F0CEC}">
   <dimension ref="A2:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -73890,4 +74144,253 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC0207-518E-48AB-8F20-B65106DCAA7A}">
+  <dimension ref="B2:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" activeCellId="3" sqref="B3:B9 B10 B13 B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="5" width="34.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>5012</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5013</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>2745</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>5015</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>5016</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
+        <v>3185</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>5017</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>5018</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>2753</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>5019</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>5020</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>4013</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>5021</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>5022</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
+        <v>3161</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>5023</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>5024</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
+        <v>2685</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>5025</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>5026</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="11" t="s">
+        <v>5027</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>5028</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="11" t="s">
+        <v>2427</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>2268</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5030</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>5031</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>5032</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>5033</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
+        <v>5034</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>5035</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>5036</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>5037</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>5037</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>5038</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>5039</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>5039</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>2399</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>5041</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>5042</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>5042</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>5043</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>5044</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>5044</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>5045</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
+        <v>2713</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>2713</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>5046</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>5047</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>5047</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>5048</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>5049</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>5049</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>5050</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
+        <v>5051</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>5052</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>5053</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
+        <v>5054</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>5055</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>5056</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixit excercises done for 15 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/TwoThousands.xlsx
+++ b/public/docs/Excel data/TwoThousands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1B35F5-464F-47B4-BEE9-614890EE4ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F25EA8-B2FB-4C88-A147-B4734681B436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="756" windowWidth="21600" windowHeight="11232" activeTab="7" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="804" yWindow="756" windowWidth="21600" windowHeight="11232" activeTab="1" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
@@ -25100,8 +25100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA00D292-BF8B-4F4B-B7D2-0977FA8E2544}">
   <dimension ref="A1:F2192"/>
   <sheetViews>
-    <sheetView topLeftCell="A1983" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1988" sqref="G1988"/>
+    <sheetView tabSelected="1" topLeftCell="A493" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B508" sqref="B508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74150,7 +74150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC0207-518E-48AB-8F20-B65106DCAA7A}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" activeCellId="3" sqref="B3:B9 B10 B13 B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixit dome for 25 lessons
</commit_message>
<xml_diff>
--- a/public/docs/Excel data/TwoThousands.xlsx
+++ b/public/docs/Excel data/TwoThousands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\Excel data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F25EA8-B2FB-4C88-A147-B4734681B436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F3DCF3-DB22-4F09-AFE7-E6AC90A59E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="756" windowWidth="21600" windowHeight="11232" activeTab="1" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21600" windowHeight="11232" activeTab="7" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11716" uniqueCount="5057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11800" uniqueCount="5096">
   <si>
     <t>з</t>
   </si>
@@ -15318,6 +15318,123 @@
   </si>
   <si>
     <t>явище – явища</t>
+  </si>
+  <si>
+    <t>Infinitive (V1)</t>
+  </si>
+  <si>
+    <t>Past Simple (V2)</t>
+  </si>
+  <si>
+    <t>Past Participle (V3)</t>
+  </si>
+  <si>
+    <t>was/were</t>
+  </si>
+  <si>
+    <t>did</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>said</t>
+  </si>
+  <si>
+    <t>went</t>
+  </si>
+  <si>
+    <t>gone</t>
+  </si>
+  <si>
+    <t>іти</t>
+  </si>
+  <si>
+    <t>got</t>
+  </si>
+  <si>
+    <t>got/gotten (AmE)</t>
+  </si>
+  <si>
+    <t>отримувати</t>
+  </si>
+  <si>
+    <t>made</t>
+  </si>
+  <si>
+    <t>робити, створювати</t>
+  </si>
+  <si>
+    <t>knew</t>
+  </si>
+  <si>
+    <t>took</t>
+  </si>
+  <si>
+    <t>taken</t>
+  </si>
+  <si>
+    <t>брати</t>
+  </si>
+  <si>
+    <t>saw</t>
+  </si>
+  <si>
+    <t>seen</t>
+  </si>
+  <si>
+    <t>бачити</t>
+  </si>
+  <si>
+    <t>came</t>
+  </si>
+  <si>
+    <t>приходити</t>
+  </si>
+  <si>
+    <t>found</t>
+  </si>
+  <si>
+    <t>знаходити</t>
+  </si>
+  <si>
+    <t>gave</t>
+  </si>
+  <si>
+    <t>given</t>
+  </si>
+  <si>
+    <t>давати</t>
+  </si>
+  <si>
+    <t>told</t>
+  </si>
+  <si>
+    <t>became</t>
+  </si>
+  <si>
+    <t>ставати</t>
+  </si>
+  <si>
+    <t>showed</t>
+  </si>
+  <si>
+    <t>shown</t>
+  </si>
+  <si>
+    <t>показувати</t>
+  </si>
+  <si>
+    <t>залишати</t>
+  </si>
+  <si>
+    <t>felt</t>
+  </si>
+  <si>
+    <t>brought</t>
+  </si>
+  <si>
+    <t>приносити</t>
   </si>
 </sst>
 </file>
@@ -25100,7 +25217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA00D292-BF8B-4F4B-B7D2-0977FA8E2544}">
   <dimension ref="A1:F2192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A493" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A493" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B508" sqref="B508"/>
     </sheetView>
   </sheetViews>
@@ -74148,10 +74265,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC0207-518E-48AB-8F20-B65106DCAA7A}">
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" activeCellId="3" sqref="B3:B9 B10 B13 B15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74324,7 +74441,7 @@
         <v>5043</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>5044</v>
       </c>
@@ -74335,7 +74452,7 @@
         <v>5045</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>2713</v>
       </c>
@@ -74346,7 +74463,7 @@
         <v>5046</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>5047</v>
       </c>
@@ -74357,7 +74474,7 @@
         <v>5048</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>5049</v>
       </c>
@@ -74368,7 +74485,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>5051</v>
       </c>
@@ -74379,7 +74496,7 @@
         <v>5053</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>5054</v>
       </c>
@@ -74388,6 +74505,300 @@
       </c>
       <c r="D22" s="11" t="s">
         <v>5056</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>5057</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>5058</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>5059</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="11" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>5060</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>2303</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>2240</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>2360</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>2360</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
+        <v>2265</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>5061</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>5062</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
+        <v>2472</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>5063</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>5063</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>5064</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>5065</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>5066</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>5067</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>5068</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>5069</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>5070</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>5070</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>5071</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="11" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>5072</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>2490</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>2718</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>2718</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>4706</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="11" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>5073</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>5074</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>5075</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
+        <v>2299</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>5076</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>5077</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>5078</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>5079</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>2406</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
+        <v>2325</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>5081</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>5081</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>5082</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
+        <v>2398</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>5083</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>5084</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>5085</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
+        <v>2781</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>5086</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>5086</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="11" t="s">
+        <v>2384</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>5087</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>2384</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>5088</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="11" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>5089</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>5090</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>5091</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="11" t="s">
+        <v>2862</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>2545</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>2545</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>5092</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="11" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>5093</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>5093</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="11" t="s">
+        <v>2739</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>5094</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>5094</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>5095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>